<commit_message>
switch Parents with NatlDirectory
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-contactpoint-viaintermediary.xlsx
+++ b/output/StructureDefinition-contactpoint-viaintermediary.xlsx
@@ -45,7 +45,7 @@
     <t>Title</t>
   </si>
   <si>
-    <t>NatlDir Contactpoint Viaintermediary</t>
+    <t>NatlDirEndpointQry Contactpoint Viaintermediary</t>
   </si>
   <si>
     <t>Status</t>
@@ -357,7 +357,7 @@
     <t>Y</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/fhir-directory-query/StructureDefinition/NatlDir-PractitionerRole|http://hl7.org/fhir/us/fhir-directory-query/StructureDefinition/NatlDir-Organization|http://hl7.org/fhir/us/fhir-directory-query/StructureDefinition/NatlDir-OrganizationAffiliation|http://hl7.org/fhir/us/fhir-directory-query/StructureDefinition/NatlDir-Location)
+    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/fhir-directory-query/StructureDefinition/NatlDirEndpointQry-PractitionerRole|http://hl7.org/fhir/us/fhir-directory-query/StructureDefinition/NatlDirEndpointQry-Organization|http://hl7.org/fhir/us/fhir-directory-query/StructureDefinition/NatlDirEndpointQry-OrganizationAffiliation|http://hl7.org/fhir/us/fhir-directory-exchange/StructureDefinition/NatlDir-Location)
 </t>
   </si>
   <si>

</xml_diff>